<commit_message>
Separate GSheet for each Product Type
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansDavinChristian\#Hans\Projects\Traveloka\UiPath\Sprint 2\Traveloka_DataAutomation_Dispatcher_Email\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 2\Traveloka_DataAutomation_Dispatcher_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC23621F-F177-458C-BFFE-FCB3BA3330B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C83B7-3E5A-4ED0-A12B-199FC6C837E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>SheetIdConfigAccomodation</t>
+  </si>
+  <si>
+    <t>SheetIdConfigTransport</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Accommodation</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
   </si>
 </sst>
 </file>
@@ -577,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2833,14 +2845,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
@@ -2921,8 +2933,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3918,5 +3944,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed typo config accommodation
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 2\Traveloka_DataAutomation_Dispatcher_Email_S2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C83B7-3E5A-4ED0-A12B-199FC6C837E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B6A43-1661-4F21-B522-39B3AF914FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>SheetIdConfigAccomodation</t>
-  </si>
-  <si>
     <t>SheetIdConfigTransport</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
+    <t>SheetIdConfigAccommodation</t>
   </si>
 </sst>
 </file>
@@ -2935,18 +2935,18 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>